<commit_message>
Update the knowledge point
</commit_message>
<xml_diff>
--- a/src/main/scala/com/nielsen/scala/knowledge point.xlsx
+++ b/src/main/scala/com/nielsen/scala/knowledge point.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="19440" windowHeight="6180"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16410" windowHeight="6600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>知识点</t>
   </si>
@@ -133,6 +133,14 @@
   </si>
   <si>
     <t>status</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>close</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>close</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -144,7 +152,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -174,6 +182,12 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -243,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -254,6 +268,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,7 +569,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -598,7 +613,9 @@
       <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
@@ -610,7 +627,9 @@
       <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="10" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">

</xml_diff>

<commit_message>
add chapter partial applied function.
</commit_message>
<xml_diff>
--- a/src/main/scala/com/nielsen/scala/knowledge point.xlsx
+++ b/src/main/scala/com/nielsen/scala/knowledge point.xlsx
@@ -11,12 +11,11 @@
     <sheet name="Q&amp;A" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:L18"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>知识点</t>
   </si>
@@ -133,6 +132,10 @@
   </si>
   <si>
     <t>status</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>close</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -574,7 +577,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:D8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -688,7 +691,9 @@
       <c r="C8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="10" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">

</xml_diff>